<commit_message>
added the structure and the VP
</commit_message>
<xml_diff>
--- a/Verification Plan/VP.xlsx
+++ b/Verification Plan/VP.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\GP\Tinyalu\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\college\GP\Mini-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{005E2C05-267C-4C39-AB88-D48D56737235}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7DE79473-B834-441E-98E1-FB8172F7F7F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VP" sheetId="1" r:id="rId1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="50">
   <si>
     <t>Label</t>
   </si>
@@ -43,12 +43,6 @@
     <t>Functionality Check</t>
   </si>
   <si>
-    <t>ADD</t>
-  </si>
-  <si>
-    <t>ADD_1</t>
-  </si>
-  <si>
     <t>Reset</t>
   </si>
   <si>
@@ -61,91 +55,13 @@
     <t>When the active low reset signal reset_n is asserted, all internal registers  must be cleared, including result, done, done1, done2, done3, a_int, b_int, mult1, and mult2.</t>
   </si>
   <si>
-    <t>ADD_2</t>
-  </si>
-  <si>
-    <t>ADD_3</t>
-  </si>
-  <si>
-    <t>AND</t>
-  </si>
-  <si>
-    <t>XOR</t>
-  </si>
-  <si>
-    <t>MULT</t>
-  </si>
-  <si>
-    <t>AND_1</t>
-  </si>
-  <si>
-    <t>XOR_1</t>
-  </si>
-  <si>
-    <t>When the opcode selects the addition operation and both operands are randomized, the output must be equal to addition of both operands.</t>
-  </si>
-  <si>
-    <t>MULT_1</t>
-  </si>
-  <si>
-    <t>MULT_2</t>
-  </si>
-  <si>
-    <t>MULT_3</t>
-  </si>
-  <si>
-    <t>When the opcode selects the addition operation and both operands are at their minimum values(0), the output must be equal to addition of both operands (0).</t>
-  </si>
-  <si>
-    <t>When the opcode selects the addition operation and both operands are at their maximum values(255), the output must be equal to addition of both operands (510).</t>
-  </si>
-  <si>
-    <t>When the opcode selects the multiplication operation and both operands are at their maximum values(255), the output must be equal to multiplication of both operands (65,025).</t>
-  </si>
-  <si>
-    <t>When the opcode selects the multiplication operation and both operands are at their minimum values(0), the output must be equal to multiplication of both operands (0).</t>
-  </si>
-  <si>
     <t>All operations</t>
   </si>
   <si>
-    <t>When the opcode selects the multiplication operation and both operands are randomized, the output must be equal to multiplication of both operands.</t>
-  </si>
-  <si>
     <t>Feature</t>
   </si>
   <si>
     <t>ALU_1</t>
-  </si>
-  <si>
-    <t>When the opcode selects the and operation AND both operands are randomized, the output must be equal to the bitwise AND of both operands .</t>
-  </si>
-  <si>
-    <t>When the opcode selects the and operation XOR both operands are randomized, the output must be equal to the bitwise XOR of both operands .</t>
-  </si>
-  <si>
-    <t>A directed opcode is applied for the addition operation, and the operands are set to their maximum values.</t>
-  </si>
-  <si>
-    <t>A directed opcode is applied for the addition operation, and the operands are set to their minimum values.</t>
-  </si>
-  <si>
-    <t>A directed opcode is applied for the addition operation, and the operands are randomized.</t>
-  </si>
-  <si>
-    <t>A directed opcode is applied for the AND operation, and the operands are randomized.</t>
-  </si>
-  <si>
-    <t>A directed opcode is applied for the XOR operation, and the operands are randomized.</t>
-  </si>
-  <si>
-    <t>All inputs are randomized.</t>
-  </si>
-  <si>
-    <t>A directed opcode is applied for the multiplication operation, and the operands are set to their maximum values.</t>
-  </si>
-  <si>
-    <t>A directed opcode is applied for the multiplication operation, and the operands are set to their minimum values.</t>
   </si>
   <si>
     <t>A directed opcode is applied for the multiplication operation, and the operands are randomized.</t>
@@ -188,9 +104,6 @@
     <t>Random</t>
   </si>
   <si>
-    <t>When the opcode selects single cycle operation and both operands are randomized, the output must be equal to the expected result.</t>
-  </si>
-  <si>
     <t>@(posedge clk) disable iff (!reset_n) start &amp;&amp; (opcode[2] == 0) &amp;&amp; (opcode != 3'b000) |=&gt; done == 1;</t>
   </si>
   <si>
@@ -230,9 +143,6 @@
     <t>When the opcode selects the multiplication operation, and in the next clock cycle another operation is selected.</t>
   </si>
   <si>
-    <t>illegal coverage bin</t>
-  </si>
-  <si>
     <t>The reset behavior is verified using immediate assertion.</t>
   </si>
   <si>
@@ -562,13 +472,30 @@
   </si>
   <si>
     <t>@(posedge clk) disable iff (!reset_n) start &amp;&amp; (opcode[2] == 0) &amp;&amp; (opcode != 3'b000) |=&gt; start == 0</t>
+  </si>
+  <si>
+    <t>The testbench uses a scoreboard to check that the output matches the expected result and assertion on different operations.</t>
+  </si>
+  <si>
+    <t>When the opcode selects single cycle or three cycles operation and both operands are randomized, the output must be equal to the expected result.</t>
+  </si>
+  <si>
+    <t>All inputs are randomized, with the operands contrained to Max_Pos or Zero most of the time, and the reset and the start signals are High most of the time.</t>
+  </si>
+  <si>
+    <t>Start_c coverage bin
+A and B Max and Min coverage bins
+op coverage bin for all operations</t>
+  </si>
+  <si>
+    <t>-</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -750,7 +677,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -764,7 +691,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -786,6 +712,45 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -795,54 +760,9 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1132,365 +1052,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView zoomScale="92" workbookViewId="0">
-      <selection activeCell="F21" sqref="F21"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="14.77734375" customWidth="1"/>
     <col min="3" max="3" width="47.44140625" customWidth="1"/>
-    <col min="4" max="4" width="36.33203125" customWidth="1"/>
-    <col min="5" max="5" width="20.21875" customWidth="1"/>
+    <col min="4" max="4" width="42.33203125" customWidth="1"/>
+    <col min="5" max="5" width="26" customWidth="1"/>
     <col min="6" max="6" width="26.77734375" customWidth="1"/>
     <col min="8" max="8" width="3.44140625" customWidth="1"/>
     <col min="9" max="9" width="11" customWidth="1"/>
     <col min="10" max="10" width="12.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="22.8" customHeight="1">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:6" ht="22.8" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="7" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="26"/>
+      <c r="C2" s="26"/>
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="27"/>
+    </row>
+    <row r="3" spans="1:6" ht="59.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="26"/>
+      <c r="D4" s="26"/>
+      <c r="E4" s="26"/>
+      <c r="F4" s="27"/>
+    </row>
+    <row r="5" spans="1:6" ht="60" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C5" s="4" t="s">
+        <v>46</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="29" t="s">
+        <v>48</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A6" s="25" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
+      <c r="E6" s="26"/>
+      <c r="F6" s="27"/>
+    </row>
+    <row r="7" spans="1:6" ht="36.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" s="16" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="8" t="s">
-        <v>1</v>
-      </c>
-      <c r="D1" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
-      <c r="A2" s="13" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="14"/>
-      <c r="C2" s="14"/>
-      <c r="D2" s="14"/>
-      <c r="E2" s="14"/>
-      <c r="F2" s="15"/>
-    </row>
-    <row r="3" spans="1:6" ht="48">
-      <c r="A3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C3" s="17" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>9</v>
-      </c>
-      <c r="E3" s="16" t="s">
-        <v>48</v>
-      </c>
-      <c r="F3" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="13" t="s">
-        <v>5</v>
-      </c>
-      <c r="B4" s="14"/>
-      <c r="C4" s="14"/>
-      <c r="D4" s="14"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
-    </row>
-    <row r="5" spans="1:6" ht="36.6">
-      <c r="A5" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B5" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C5" s="17" t="s">
+      <c r="F7" s="8" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" ht="24" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="E5" s="19"/>
-      <c r="F5" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" ht="36.6">
-      <c r="A6" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B6" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="C6" s="17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>33</v>
-      </c>
-      <c r="E6" s="19"/>
-      <c r="F6" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" ht="36.6">
-      <c r="A7" s="1" t="s">
+      <c r="C8" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="D8" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C7" s="17" t="s">
-        <v>18</v>
-      </c>
-      <c r="D7" s="17" t="s">
-        <v>34</v>
-      </c>
-      <c r="E7" s="19"/>
-      <c r="F7" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
-    </row>
-    <row r="9" spans="1:6" ht="36.6">
-      <c r="A9" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C9" s="18" t="s">
+      <c r="E8" s="17" t="s">
+        <v>49</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="36" x14ac:dyDescent="0.3">
+      <c r="A9" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="D9" s="17" t="s">
-        <v>35</v>
-      </c>
-      <c r="E9" s="19"/>
-      <c r="F9" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
-      <c r="A10" s="13" t="s">
-        <v>14</v>
-      </c>
-      <c r="B10" s="14"/>
-      <c r="C10" s="14"/>
-      <c r="D10" s="14"/>
-      <c r="E10" s="14"/>
-      <c r="F10" s="15"/>
-    </row>
-    <row r="11" spans="1:6" ht="36.6">
-      <c r="A11" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B11" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>31</v>
-      </c>
-      <c r="D11" s="17" t="s">
+      <c r="B9" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D9" s="4" t="s">
         <v>36</v>
       </c>
-      <c r="E11" s="19"/>
-      <c r="F11" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
-      <c r="A12" s="13" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="14"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="15"/>
-    </row>
-    <row r="13" spans="1:6" ht="36.6">
-      <c r="A13" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B13" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C13" s="17" t="s">
-        <v>24</v>
-      </c>
-      <c r="D13" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="E13" s="19"/>
-      <c r="F13" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="36.6">
-      <c r="A14" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="B14" s="20" t="s">
-        <v>50</v>
-      </c>
-      <c r="C14" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="D14" s="18" t="s">
+      <c r="E9" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="15" t="s">
         <v>39</v>
       </c>
-      <c r="E14" s="19"/>
-      <c r="F14" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="36.6">
-      <c r="A15" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="B15" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C15" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E15" s="19"/>
-      <c r="F15" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
-      <c r="A16" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="B16" s="14"/>
-      <c r="C16" s="14"/>
-      <c r="D16" s="14"/>
-      <c r="E16" s="14"/>
-      <c r="F16" s="15"/>
-    </row>
-    <row r="17" spans="1:6" ht="36.6">
-      <c r="A17" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B17" s="12" t="s">
-        <v>52</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>53</v>
-      </c>
-      <c r="D17" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="E17" s="5"/>
-      <c r="F17" s="10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="15"/>
-    </row>
-    <row r="19" spans="1:6" ht="36.6">
-      <c r="A19" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="B19" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>62</v>
-      </c>
-      <c r="D19" s="17" t="s">
-        <v>63</v>
-      </c>
-      <c r="E19" s="23" t="s">
-        <v>67</v>
-      </c>
-      <c r="F19" s="9" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" ht="24">
-      <c r="A20" s="1" t="s">
-        <v>58</v>
-      </c>
-      <c r="B20" s="16" t="s">
-        <v>51</v>
-      </c>
-      <c r="C20" s="17" t="s">
-        <v>64</v>
-      </c>
-      <c r="D20" s="17" t="s">
-        <v>40</v>
-      </c>
-      <c r="E20" s="24" t="s">
-        <v>67</v>
-      </c>
-      <c r="F20" s="2" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" ht="36">
-      <c r="A21" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B21" s="21" t="s">
-        <v>51</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="D21" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="E21" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="F21" s="22" t="s">
-        <v>69</v>
-      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A10" s="28"/>
+      <c r="B10" s="28"/>
+      <c r="C10" s="28"/>
+      <c r="D10" s="28"/>
+      <c r="E10" s="28"/>
+      <c r="F10" s="28"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="28"/>
+      <c r="B11" s="28"/>
+      <c r="C11" s="28"/>
+      <c r="D11" s="28"/>
+      <c r="E11" s="28"/>
+      <c r="F11" s="28"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A12" s="28"/>
+      <c r="B12" s="28"/>
+      <c r="C12" s="28"/>
+      <c r="D12" s="28"/>
+      <c r="E12" s="28"/>
+      <c r="F12" s="28"/>
     </row>
   </sheetData>
-  <mergeCells count="7">
-    <mergeCell ref="A18:F18"/>
-    <mergeCell ref="A16:F16"/>
+  <mergeCells count="6">
+    <mergeCell ref="A6:F6"/>
+    <mergeCell ref="A4:F4"/>
     <mergeCell ref="A2:F2"/>
-    <mergeCell ref="A4:F4"/>
-    <mergeCell ref="A8:F8"/>
     <mergeCell ref="A10:F10"/>
     <mergeCell ref="A12:F12"/>
+    <mergeCell ref="A11:F11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1501,78 +1262,78 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A3098DA2-B117-41AA-8A2E-E10E5C0FA9DE}">
   <dimension ref="A1:B8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="59.21875" customWidth="1"/>
     <col min="2" max="2" width="65.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="23.4" customHeight="1">
-      <c r="A1" s="11" t="s">
-        <v>28</v>
-      </c>
-      <c r="B1" s="11" t="s">
+    <row r="1" spans="1:2" ht="23.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B1" s="10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A2" s="18" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="19" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A3" s="18" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="20" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="21" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="43.8" x14ac:dyDescent="0.3">
+      <c r="A5" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="B5" s="20" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" ht="43.8" x14ac:dyDescent="0.3">
+      <c r="A6" s="22" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" ht="27.6">
-      <c r="A2" s="25" t="s">
+      <c r="B6" s="20" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="18" t="s">
         <v>43</v>
       </c>
-      <c r="B2" s="26" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="27.6">
-      <c r="A3" s="25" t="s">
-        <v>46</v>
-      </c>
-      <c r="B3" s="27" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="25" t="s">
-        <v>44</v>
-      </c>
-      <c r="B4" s="28" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="41.4">
-      <c r="A5" s="29" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="41.4">
-      <c r="A6" s="29" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="27" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="27.6">
-      <c r="A7" s="30" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="27" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="27.6">
-      <c r="A8" s="31" t="s">
-        <v>61</v>
-      </c>
-      <c r="B8" s="32" t="s">
-        <v>60</v>
+      <c r="B7" s="20" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" ht="27.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="23" t="s">
+        <v>32</v>
+      </c>
+      <c r="B8" s="24" t="s">
+        <v>31</v>
       </c>
     </row>
   </sheetData>

</xml_diff>